<commit_message>
bms id bug fix
</commit_message>
<xml_diff>
--- a/Results.xlsx
+++ b/Results.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -467,11 +467,11 @@
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>792</v>
+        <v>805</v>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>No results</t>
+          <t>NO Tname and no Bname</t>
         </is>
       </c>
     </row>
@@ -487,11 +487,11 @@
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>1258</v>
+        <v>965</v>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Genetically Modified Declaration Code</t>
+          <t>NO Tname and no Bname</t>
         </is>
       </c>
     </row>

</xml_diff>